<commit_message>
Working summary page implemented
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53718360-4262-46BF-9993-700067E70EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908909A-76E1-4112-9878-6EF85EC6D4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="22540" windowHeight="14320" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="AF2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1035,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added download button and formatted as percent and currency
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908909A-76E1-4112-9878-6EF85EC6D4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFF2AD6-8136-4169-89D8-5C4804AD1BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="0" windowWidth="22540" windowHeight="14320" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="180" yWindow="1125" windowWidth="22905" windowHeight="10530" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="204">
   <si>
     <t>tab_name</t>
   </si>
@@ -642,13 +642,22 @@
   </si>
   <si>
     <t>accordion_text</t>
+  </si>
+  <si>
+    <t>value_format</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>currency_per_capita</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,6 +667,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -698,6 +715,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="F49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,42 +1069,46 @@
     <col min="5" max="5" width="95.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.26953125" customWidth="1"/>
     <col min="7" max="7" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="81.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" customWidth="1"/>
+    <col min="9" max="10" width="81.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1104,11 +1130,11 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1130,11 +1156,14 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1156,11 +1185,11 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1182,11 +1211,11 @@
       <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1208,11 +1237,11 @@
       <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1234,11 +1263,11 @@
       <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1260,11 +1289,14 @@
       <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1286,11 +1318,14 @@
       <c r="G9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1312,11 +1347,14 @@
       <c r="G10" t="s">
         <v>35</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I10" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1338,11 +1376,14 @@
       <c r="G11" t="s">
         <v>36</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1364,11 +1405,14 @@
       <c r="G12" t="s">
         <v>36</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1390,11 +1434,14 @@
       <c r="G13" t="s">
         <v>36</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I13" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1416,11 +1463,14 @@
       <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1442,11 +1492,14 @@
       <c r="G15" t="s">
         <v>47</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1468,11 +1521,14 @@
       <c r="G16" t="s">
         <v>47</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I16" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1494,11 +1550,12 @@
       <c r="G17" t="s">
         <v>46</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1520,11 +1577,12 @@
       <c r="G18" t="s">
         <v>46</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="1"/>
+      <c r="I18" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1546,11 +1604,12 @@
       <c r="G19" t="s">
         <v>46</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="1"/>
+      <c r="I19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1572,11 +1631,14 @@
       <c r="G20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I20" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1598,11 +1660,14 @@
       <c r="G21" t="s">
         <v>53</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I21" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1624,11 +1689,14 @@
       <c r="G22" t="s">
         <v>58</v>
       </c>
-      <c r="H22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1650,11 +1718,14 @@
       <c r="G23" t="s">
         <v>61</v>
       </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1676,11 +1747,11 @@
       <c r="G24" t="s">
         <v>21</v>
       </c>
-      <c r="H24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1702,17 +1773,17 @@
       <c r="G25" t="s">
         <v>21</v>
       </c>
-      <c r="H25" t="s">
-        <v>13</v>
-      </c>
       <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" t="s">
         <v>140</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1734,17 +1805,17 @@
       <c r="G26" t="s">
         <v>21</v>
       </c>
-      <c r="H26" t="s">
-        <v>13</v>
-      </c>
       <c r="I26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" t="s">
         <v>141</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1766,17 +1837,17 @@
       <c r="G27" t="s">
         <v>21</v>
       </c>
-      <c r="H27" t="s">
-        <v>13</v>
-      </c>
       <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" t="s">
         <v>142</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1798,17 +1869,17 @@
       <c r="G28" t="s">
         <v>21</v>
       </c>
-      <c r="H28" t="s">
-        <v>13</v>
-      </c>
       <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" t="s">
         <v>143</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1830,17 +1901,17 @@
       <c r="G29" t="s">
         <v>21</v>
       </c>
-      <c r="H29" t="s">
-        <v>13</v>
-      </c>
       <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
         <v>144</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1862,17 +1933,17 @@
       <c r="G30" t="s">
         <v>21</v>
       </c>
-      <c r="H30" t="s">
-        <v>13</v>
-      </c>
       <c r="I30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
         <v>145</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1894,17 +1965,17 @@
       <c r="G31" t="s">
         <v>21</v>
       </c>
-      <c r="H31" t="s">
-        <v>13</v>
-      </c>
       <c r="I31" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" t="s">
         <v>146</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1926,17 +1997,17 @@
       <c r="G32" t="s">
         <v>21</v>
       </c>
-      <c r="H32" t="s">
-        <v>13</v>
-      </c>
       <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
         <v>147</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1958,17 +2029,17 @@
       <c r="G33" t="s">
         <v>21</v>
       </c>
-      <c r="H33" t="s">
-        <v>13</v>
-      </c>
       <c r="I33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" t="s">
         <v>148</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1990,17 +2061,17 @@
       <c r="G34" t="s">
         <v>21</v>
       </c>
-      <c r="H34" t="s">
-        <v>13</v>
-      </c>
       <c r="I34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" t="s">
         <v>149</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2022,17 +2093,17 @@
       <c r="G35" t="s">
         <v>21</v>
       </c>
-      <c r="H35" t="s">
-        <v>13</v>
-      </c>
       <c r="I35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" t="s">
         <v>150</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2054,17 +2125,17 @@
       <c r="G36" t="s">
         <v>21</v>
       </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
       <c r="I36" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" t="s">
         <v>151</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2086,17 +2157,17 @@
       <c r="G37" t="s">
         <v>21</v>
       </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
       <c r="I37" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" t="s">
         <v>138</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2118,17 +2189,17 @@
       <c r="G38" t="s">
         <v>21</v>
       </c>
-      <c r="H38" t="s">
-        <v>13</v>
-      </c>
       <c r="I38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" t="s">
         <v>135</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2150,17 +2221,17 @@
       <c r="G39" t="s">
         <v>21</v>
       </c>
-      <c r="H39" t="s">
-        <v>13</v>
-      </c>
       <c r="I39" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" t="s">
         <v>137</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2182,17 +2253,17 @@
       <c r="G40" t="s">
         <v>21</v>
       </c>
-      <c r="H40" t="s">
-        <v>13</v>
-      </c>
       <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" t="s">
         <v>134</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2214,17 +2285,17 @@
       <c r="G41" t="s">
         <v>21</v>
       </c>
-      <c r="H41" t="s">
-        <v>13</v>
-      </c>
       <c r="I41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" t="s">
         <v>136</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2246,14 +2317,17 @@
       <c r="G42" t="s">
         <v>73</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I42" t="s">
         <v>183</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2275,14 +2349,17 @@
       <c r="G43" t="s">
         <v>53</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" t="s">
         <v>184</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2304,14 +2381,14 @@
       <c r="G44" t="s">
         <v>93</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>185</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2333,14 +2410,17 @@
       <c r="G45" t="s">
         <v>53</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I45" t="s">
         <v>186</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2362,14 +2442,17 @@
       <c r="G46" t="s">
         <v>53</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I46" t="s">
         <v>199</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2391,14 +2474,17 @@
       <c r="G47" t="s">
         <v>53</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" t="s">
         <v>187</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2420,14 +2506,17 @@
       <c r="G48" t="s">
         <v>53</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I48" t="s">
         <v>188</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2449,14 +2538,17 @@
       <c r="G49" t="s">
         <v>53</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I49" t="s">
         <v>189</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2478,14 +2570,17 @@
       <c r="G50" t="s">
         <v>53</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I50" t="s">
         <v>190</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2507,14 +2602,17 @@
       <c r="G51" t="s">
         <v>53</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I51" t="s">
         <v>191</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2536,14 +2634,17 @@
       <c r="G52" t="s">
         <v>100</v>
       </c>
-      <c r="H52" t="s">
-        <v>13</v>
+      <c r="H52" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I52" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2565,14 +2666,17 @@
       <c r="G53" t="s">
         <v>103</v>
       </c>
-      <c r="H53" t="s">
-        <v>13</v>
+      <c r="H53" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2594,14 +2698,17 @@
       <c r="G54" t="s">
         <v>105</v>
       </c>
-      <c r="H54" t="s">
-        <v>13</v>
+      <c r="H54" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2623,14 +2730,14 @@
       <c r="G55" t="s">
         <v>132</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>192</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2652,14 +2759,14 @@
       <c r="G56" t="s">
         <v>132</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>193</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2681,14 +2788,14 @@
       <c r="G57" t="s">
         <v>132</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>194</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2710,14 +2817,14 @@
       <c r="G58" t="s">
         <v>132</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>195</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2739,14 +2846,17 @@
       <c r="G59" t="s">
         <v>121</v>
       </c>
-      <c r="H59" t="s">
-        <v>13</v>
+      <c r="H59" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2768,14 +2878,17 @@
       <c r="G60" t="s">
         <v>123</v>
       </c>
-      <c r="H60" t="s">
-        <v>13</v>
+      <c r="H60" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2797,14 +2910,17 @@
       <c r="G61" t="s">
         <v>124</v>
       </c>
-      <c r="H61" t="s">
-        <v>13</v>
+      <c r="H61" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2826,14 +2942,15 @@
       <c r="G62" t="s">
         <v>127</v>
       </c>
-      <c r="H62" t="s">
-        <v>13</v>
-      </c>
+      <c r="H62" s="1"/>
       <c r="I62" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2855,10 +2972,13 @@
       <c r="G63" t="s">
         <v>131</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I63" t="s">
         <v>196</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added stat neighbours for ethnicity, spending, ofsted ratings.  UASC not displaying still. Fixed some styling
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFF2AD6-8136-4169-89D8-5C4804AD1BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD63EC0-A044-4FBC-A284-06AB4F51446F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1125" windowWidth="22905" windowHeight="10530" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="AF2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="199">
   <si>
     <t>tab_name</t>
   </si>
@@ -374,21 +375,6 @@
     <t>Number of local authorities with an Ofsted Leadership Rating of Inadequate</t>
   </si>
   <si>
-    <t>ofsted_leadership_data_long</t>
-  </si>
-  <si>
-    <t>list(Rating="inadequate_count")</t>
-  </si>
-  <si>
-    <t>list(Rating="requires_improvement_count")</t>
-  </si>
-  <si>
-    <t>list(Rating="good_count")</t>
-  </si>
-  <si>
-    <t>list(Rating="outstanding_count")</t>
-  </si>
-  <si>
     <t>Enabler: The workforce is equipped and effective.</t>
   </si>
   <si>
@@ -437,9 +423,6 @@
     <t>inpost_headcount_percentage</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>list(role = "Total", breakdown = "White")</t>
   </si>
   <si>
@@ -617,18 +600,6 @@
     <t>list(age = '19 to 21 years', accommodation_suitability = 'Accommodation considered suitable')</t>
   </si>
   <si>
-    <t>list(Rating='inadequate_count')</t>
-  </si>
-  <si>
-    <t>list(Rating='good_count')</t>
-  </si>
-  <si>
-    <t>list(Rating='requires_improvement_count')</t>
-  </si>
-  <si>
-    <t>list(Rating='outstanding_count')</t>
-  </si>
-  <si>
     <t>list(role = 'Total', breakdown = 'White')</t>
   </si>
   <si>
@@ -651,6 +622,21 @@
   </si>
   <si>
     <t>currency_per_capita</t>
+  </si>
+  <si>
+    <t>ofsted_leadership_data</t>
+  </si>
+  <si>
+    <t>outstanding_count</t>
+  </si>
+  <si>
+    <t>good_count</t>
+  </si>
+  <si>
+    <t>requires_improvement_count</t>
+  </si>
+  <si>
+    <t>inadequate_count</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1096,16 +1082,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1157,7 +1143,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -1186,7 +1172,7 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1212,7 +1198,7 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1238,7 +1224,7 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1264,7 +1250,7 @@
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1290,10 +1276,10 @@
         <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1319,10 +1305,10 @@
         <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1348,10 +1334,10 @@
         <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1377,10 +1363,10 @@
         <v>36</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1406,10 +1392,10 @@
         <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1435,10 +1421,10 @@
         <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I13" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1464,10 +1450,10 @@
         <v>47</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I14" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1493,10 +1479,10 @@
         <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1522,10 +1508,10 @@
         <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I16" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1552,7 +1538,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1579,7 +1565,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1606,7 +1592,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1632,10 +1618,10 @@
         <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1661,10 +1647,10 @@
         <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1690,7 +1676,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1719,7 +1705,7 @@
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1762,13 +1748,13 @@
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
@@ -1777,10 +1763,10 @@
         <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -1794,13 +1780,13 @@
         <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
@@ -1809,10 +1795,10 @@
         <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1826,13 +1812,13 @@
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F27" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
@@ -1841,10 +1827,10 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K27" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -1858,13 +1844,13 @@
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F28" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -1873,10 +1859,10 @@
         <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K28" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1890,13 +1876,13 @@
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G29" t="s">
         <v>21</v>
@@ -1905,10 +1891,10 @@
         <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="K29" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -1922,13 +1908,13 @@
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="F30" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G30" t="s">
         <v>21</v>
@@ -1937,10 +1923,10 @@
         <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K30" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -1954,13 +1940,13 @@
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
@@ -1969,10 +1955,10 @@
         <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="K31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -1986,13 +1972,13 @@
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F32" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
@@ -2001,10 +1987,10 @@
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K32" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -2018,13 +2004,13 @@
         <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
@@ -2033,10 +2019,10 @@
         <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="K33" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -2050,13 +2036,13 @@
         <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G34" t="s">
         <v>21</v>
@@ -2065,10 +2051,10 @@
         <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K34" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -2082,13 +2068,13 @@
         <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F35" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G35" t="s">
         <v>21</v>
@@ -2097,10 +2083,10 @@
         <v>13</v>
       </c>
       <c r="J35" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="K35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -2114,13 +2100,13 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F36" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
@@ -2129,10 +2115,10 @@
         <v>13</v>
       </c>
       <c r="J36" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K36" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -2146,13 +2132,13 @@
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F37" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G37" t="s">
         <v>21</v>
@@ -2161,10 +2147,10 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K37" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -2178,13 +2164,13 @@
         <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F38" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
@@ -2193,10 +2179,10 @@
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K38" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -2210,13 +2196,13 @@
         <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
@@ -2225,10 +2211,10 @@
         <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="K39" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -2242,13 +2228,13 @@
         <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F40" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G40" t="s">
         <v>21</v>
@@ -2257,10 +2243,10 @@
         <v>13</v>
       </c>
       <c r="J40" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="K40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -2274,13 +2260,13 @@
         <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F41" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
@@ -2289,10 +2275,10 @@
         <v>13</v>
       </c>
       <c r="J41" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="K41" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -2318,10 +2304,10 @@
         <v>73</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I42" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="K42" t="s">
         <v>74</v>
@@ -2350,10 +2336,10 @@
         <v>53</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I43" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K43" t="s">
         <v>77</v>
@@ -2382,7 +2368,7 @@
         <v>93</v>
       </c>
       <c r="I44" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="K44" t="s">
         <v>85</v>
@@ -2411,10 +2397,10 @@
         <v>53</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I45" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="K45" t="s">
         <v>76</v>
@@ -2443,10 +2429,10 @@
         <v>53</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I46" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="K46" t="s">
         <v>78</v>
@@ -2475,10 +2461,10 @@
         <v>53</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I47" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="K47" t="s">
         <v>79</v>
@@ -2507,10 +2493,10 @@
         <v>53</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I48" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K48" t="s">
         <v>87</v>
@@ -2539,10 +2525,10 @@
         <v>53</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I49" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K49" t="s">
         <v>88</v>
@@ -2571,10 +2557,10 @@
         <v>53</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I50" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="K50" t="s">
         <v>92</v>
@@ -2603,10 +2589,10 @@
         <v>53</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I51" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K51" t="s">
         <v>91</v>
@@ -2635,7 +2621,7 @@
         <v>100</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I52" t="s">
         <v>13</v>
@@ -2667,7 +2653,7 @@
         <v>103</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2699,7 +2685,7 @@
         <v>105</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2725,16 +2711,16 @@
         <v>106</v>
       </c>
       <c r="F55" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="G55" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="I55" t="s">
-        <v>192</v>
+        <v>13</v>
       </c>
       <c r="J55" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -2754,16 +2740,16 @@
         <v>108</v>
       </c>
       <c r="F56" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="G56" t="s">
-        <v>132</v>
+        <v>196</v>
       </c>
       <c r="I56" t="s">
-        <v>193</v>
+        <v>13</v>
       </c>
       <c r="J56" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
@@ -2783,16 +2769,16 @@
         <v>109</v>
       </c>
       <c r="F57" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="G57" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="I57" t="s">
-        <v>194</v>
+        <v>13</v>
       </c>
       <c r="J57" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
@@ -2812,16 +2798,16 @@
         <v>110</v>
       </c>
       <c r="F58" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="G58" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="I58" t="s">
-        <v>195</v>
+        <v>13</v>
       </c>
       <c r="J58" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
@@ -2832,22 +2818,22 @@
         <v>94</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" t="s">
-        <v>122</v>
-      </c>
-      <c r="G59" t="s">
-        <v>121</v>
-      </c>
       <c r="H59" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2864,22 +2850,22 @@
         <v>94</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" t="s">
         <v>117</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F60" t="s">
-        <v>122</v>
-      </c>
       <c r="G60" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2896,22 +2882,22 @@
         <v>94</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" t="s">
         <v>117</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F61" t="s">
-        <v>122</v>
-      </c>
       <c r="G61" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2928,19 +2914,19 @@
         <v>94</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" t="s">
         <v>122</v>
-      </c>
-      <c r="G62" t="s">
-        <v>127</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" t="s">
@@ -2958,28 +2944,28 @@
         <v>94</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F63" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G63" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="I63" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J63" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3104,62 +3090,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3179,27 +3165,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added wellbeing SDQ with stats neighbours. Corrected sort order on Ofsted ratings. Fixed ethnicity rate plot. Updated metadata for SDQ
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD63EC0-A044-4FBC-A284-06AB4F51446F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABCEC5-5B3B-49A7-883E-329A172F6173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="51930" windowHeight="21210" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="AF2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="204">
   <si>
     <t>tab_name</t>
   </si>
@@ -637,6 +636,21 @@
   </si>
   <si>
     <t>inadequate_count</t>
+  </si>
+  <si>
+    <t>Child wellbeing</t>
+  </si>
+  <si>
+    <t>Average SDQ score</t>
+  </si>
+  <si>
+    <t>list(characteristic = 'SDQ average score')</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>wellbeing_sdq_data</t>
   </si>
 </sst>
 </file>
@@ -1040,26 +1054,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="3" max="3" width="69.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.81640625" customWidth="1"/>
-    <col min="5" max="5" width="95.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.26953125" customWidth="1"/>
-    <col min="7" max="7" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.453125" customWidth="1"/>
-    <col min="9" max="10" width="81.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" customWidth="1"/>
+    <col min="5" max="5" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="10" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1094,7 +1108,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1120,7 +1134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1149,7 +1163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1175,7 +1189,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1253,7 +1267,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1282,7 +1296,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1340,7 +1354,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1369,7 +1383,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1398,7 +1412,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1427,7 +1441,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1456,7 +1470,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1485,7 +1499,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1514,7 +1528,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1541,7 +1555,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1568,7 +1582,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1595,7 +1609,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1624,7 +1638,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1653,7 +1667,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1682,7 +1696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1711,7 +1725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1737,7 +1751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1769,7 +1783,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1801,7 +1815,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1833,7 +1847,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1865,7 +1879,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1897,7 +1911,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1929,7 +1943,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1961,7 +1975,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1993,7 +2007,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2025,7 +2039,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2057,7 +2071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2089,7 +2103,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2121,7 +2135,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2153,7 +2167,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2185,7 +2199,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2217,7 +2231,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2249,7 +2263,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2281,7 +2295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2313,7 +2327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2345,7 +2359,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2374,7 +2388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2406,7 +2420,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2438,7 +2452,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2470,7 +2484,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2481,28 +2495,23 @@
         <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F48" t="s">
-        <v>89</v>
-      </c>
-      <c r="G48" t="s">
-        <v>53</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>192</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>182</v>
-      </c>
-      <c r="K48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>80</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F49" t="s">
         <v>89</v>
@@ -2528,13 +2537,13 @@
         <v>192</v>
       </c>
       <c r="I49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2548,10 +2557,10 @@
         <v>80</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G50" t="s">
         <v>53</v>
@@ -2560,13 +2569,13 @@
         <v>192</v>
       </c>
       <c r="I50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>80</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F51" t="s">
         <v>90</v>
@@ -2592,45 +2601,45 @@
         <v>192</v>
       </c>
       <c r="I51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K51" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F52" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G52" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>192</v>
       </c>
       <c r="I52" t="s">
-        <v>13</v>
-      </c>
-      <c r="J52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+      <c r="K52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2644,16 +2653,16 @@
         <v>96</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G53" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2662,7 +2671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2676,16 +2685,16 @@
         <v>96</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2694,7 +2703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2705,16 +2714,19 @@
         <v>95</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F55" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="G55" t="s">
-        <v>195</v>
+        <v>105</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2723,7 +2735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2737,13 +2749,13 @@
         <v>107</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F56" t="s">
         <v>194</v>
       </c>
       <c r="G56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2752,7 +2764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2766,13 +2778,13 @@
         <v>107</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F57" t="s">
         <v>194</v>
       </c>
       <c r="G57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2781,7 +2793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2795,13 +2807,13 @@
         <v>107</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F58" t="s">
         <v>194</v>
       </c>
       <c r="G58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2810,7 +2822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2818,22 +2830,19 @@
         <v>94</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F59" t="s">
-        <v>117</v>
+        <v>194</v>
       </c>
       <c r="G59" t="s">
-        <v>116</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2842,7 +2851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2856,13 +2865,13 @@
         <v>112</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F60" t="s">
         <v>117</v>
       </c>
       <c r="G60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>192</v>
@@ -2874,7 +2883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2888,13 +2897,13 @@
         <v>112</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F61" t="s">
         <v>117</v>
       </c>
       <c r="G61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>192</v>
@@ -2906,7 +2915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2917,18 +2926,20 @@
         <v>111</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F62" t="s">
         <v>117</v>
       </c>
       <c r="G62" t="s">
-        <v>122</v>
-      </c>
-      <c r="H62" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="I62" t="s">
         <v>13</v>
       </c>
@@ -2936,7 +2947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2947,24 +2958,54 @@
         <v>111</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
+        <v>117</v>
+      </c>
+      <c r="G63" t="s">
+        <v>122</v>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="I63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>125</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" t="s">
         <v>126</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I64" t="s">
         <v>186</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J64" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2983,19 +3024,19 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -3021,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3047,7 +3088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3086,64 +3127,64 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -3161,29 +3202,29 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Corrected metadata for spending no cla
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BABCEC5-5B3B-49A7-883E-329A172F6173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A07E00D-BCC5-474E-9567-AC25C0781A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="51930" windowHeight="21210" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -356,9 +356,6 @@
     <t>spending_data_no_cla</t>
   </si>
   <si>
-    <t>Excluding CLA Share</t>
-  </si>
-  <si>
     <t>Number of local authorities with an Ofsted Leadership Rating of Outstanding</t>
   </si>
   <si>
@@ -651,6 +648,9 @@
   </si>
   <si>
     <t>wellbeing_sdq_data</t>
+  </si>
+  <si>
+    <t>minus_cla_share</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1096,16 +1096,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -1186,7 +1186,7 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1290,10 +1290,10 @@
         <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1319,10 +1319,10 @@
         <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1348,10 +1348,10 @@
         <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1377,10 +1377,10 @@
         <v>36</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
         <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1435,10 +1435,10 @@
         <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,10 +1464,10 @@
         <v>47</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1493,10 +1493,10 @@
         <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1522,10 +1522,10 @@
         <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,10 +1632,10 @@
         <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1661,10 +1661,10 @@
         <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1719,7 +1719,7 @@
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1762,13 +1762,13 @@
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
@@ -1777,10 +1777,10 @@
         <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,13 +1794,13 @@
         <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
@@ -1809,10 +1809,10 @@
         <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1826,13 +1826,13 @@
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
@@ -1841,10 +1841,10 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1858,13 +1858,13 @@
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -1873,10 +1873,10 @@
         <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G29" t="s">
         <v>21</v>
@@ -1905,10 +1905,10 @@
         <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1922,13 +1922,13 @@
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G30" t="s">
         <v>21</v>
@@ -1937,10 +1937,10 @@
         <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1954,13 +1954,13 @@
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
@@ -1969,10 +1969,10 @@
         <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1986,13 +1986,13 @@
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
@@ -2001,10 +2001,10 @@
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2018,13 +2018,13 @@
         <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
@@ -2033,10 +2033,10 @@
         <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2050,13 +2050,13 @@
         <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G34" t="s">
         <v>21</v>
@@ -2065,10 +2065,10 @@
         <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2082,13 +2082,13 @@
         <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G35" t="s">
         <v>21</v>
@@ -2097,10 +2097,10 @@
         <v>13</v>
       </c>
       <c r="J35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2114,13 +2114,13 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
@@ -2129,10 +2129,10 @@
         <v>13</v>
       </c>
       <c r="J36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2146,13 +2146,13 @@
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G37" t="s">
         <v>21</v>
@@ -2161,10 +2161,10 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2178,13 +2178,13 @@
         <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
@@ -2193,10 +2193,10 @@
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2210,13 +2210,13 @@
         <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
@@ -2225,10 +2225,10 @@
         <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2242,13 +2242,13 @@
         <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G40" t="s">
         <v>21</v>
@@ -2257,10 +2257,10 @@
         <v>13</v>
       </c>
       <c r="J40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2274,13 +2274,13 @@
         <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
@@ -2289,10 +2289,10 @@
         <v>13</v>
       </c>
       <c r="J41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2318,10 +2318,10 @@
         <v>73</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K42" t="s">
         <v>74</v>
@@ -2350,10 +2350,10 @@
         <v>53</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K43" t="s">
         <v>77</v>
@@ -2382,7 +2382,7 @@
         <v>93</v>
       </c>
       <c r="I44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K44" t="s">
         <v>85</v>
@@ -2411,10 +2411,10 @@
         <v>53</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K45" t="s">
         <v>76</v>
@@ -2443,10 +2443,10 @@
         <v>53</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K46" t="s">
         <v>78</v>
@@ -2475,10 +2475,10 @@
         <v>53</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K47" t="s">
         <v>79</v>
@@ -2495,20 +2495,20 @@
         <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2534,10 +2534,10 @@
         <v>53</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K49" t="s">
         <v>87</v>
@@ -2566,10 +2566,10 @@
         <v>53</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K50" t="s">
         <v>88</v>
@@ -2598,10 +2598,10 @@
         <v>53</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K51" t="s">
         <v>92</v>
@@ -2630,10 +2630,10 @@
         <v>53</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K52" t="s">
         <v>91</v>
@@ -2662,7 +2662,7 @@
         <v>100</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2694,7 +2694,7 @@
         <v>103</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2723,10 +2723,10 @@
         <v>104</v>
       </c>
       <c r="G55" t="s">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2746,16 +2746,16 @@
         <v>95</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F56" t="s">
+        <v>193</v>
+      </c>
+      <c r="G56" t="s">
         <v>194</v>
-      </c>
-      <c r="G56" t="s">
-        <v>195</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2775,16 +2775,16 @@
         <v>95</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="F57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2804,16 +2804,16 @@
         <v>95</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2833,16 +2833,16 @@
         <v>95</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2859,22 +2859,22 @@
         <v>94</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="F60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2891,22 +2891,22 @@
         <v>94</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F61" t="s">
+        <v>116</v>
+      </c>
+      <c r="G61" t="s">
         <v>117</v>
       </c>
-      <c r="G61" t="s">
-        <v>118</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2923,22 +2923,22 @@
         <v>94</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I62" t="s">
         <v>13</v>
@@ -2955,19 +2955,19 @@
         <v>94</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63" t="s">
         <v>121</v>
-      </c>
-      <c r="F63" t="s">
-        <v>117</v>
-      </c>
-      <c r="G63" t="s">
-        <v>122</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" t="s">
@@ -2985,28 +2985,28 @@
         <v>94</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F64" t="s">
         <v>124</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>125</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I64" t="s">
+        <v>185</v>
+      </c>
+      <c r="J64" t="s">
         <v>126</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="I64" t="s">
-        <v>186</v>
-      </c>
-      <c r="J64" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3131,62 +3131,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3206,27 +3206,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revided summary page export CSV, corrected ethnicity non-white stat, created stats neighbours for ethnicity non-white summary page stat.
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A07E00D-BCC5-474E-9567-AC25C0781A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F46AB-ACA6-4428-B6E2-DCB95B8A2026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
@@ -341,9 +341,6 @@
     <t>Share of children’s services spend not on CLA</t>
   </si>
   <si>
-    <t>CS Share</t>
-  </si>
-  <si>
     <t>spending_data</t>
   </si>
   <si>
@@ -419,9 +416,6 @@
     <t>inpost_headcount_percentage</t>
   </si>
   <si>
-    <t>list(role = "Total", breakdown = "White")</t>
-  </si>
-  <si>
     <t>Going missing</t>
   </si>
   <si>
@@ -596,9 +590,6 @@
     <t>list(age = '19 to 21 years', accommodation_suitability = 'Accommodation considered suitable')</t>
   </si>
   <si>
-    <t>list(role = 'Total', breakdown = 'White')</t>
-  </si>
-  <si>
     <t>assessment_factor</t>
   </si>
   <si>
@@ -651,6 +642,15 @@
   </si>
   <si>
     <t>minus_cla_share</t>
+  </si>
+  <si>
+    <t>cs_share</t>
+  </si>
+  <si>
+    <t>list(role = 'Total', breakdown = 'Non-white')</t>
+  </si>
+  <si>
+    <t>list(role = "Total", breakdown = "Non-white")</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="H33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1096,16 +1096,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -1186,7 +1186,7 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1290,10 +1290,10 @@
         <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1319,10 +1319,10 @@
         <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1348,10 +1348,10 @@
         <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1377,10 +1377,10 @@
         <v>36</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
         <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1435,10 +1435,10 @@
         <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,10 +1464,10 @@
         <v>47</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1493,10 +1493,10 @@
         <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1522,10 +1522,10 @@
         <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,10 +1632,10 @@
         <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I20" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1661,10 +1661,10 @@
         <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1719,7 +1719,7 @@
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1762,13 +1762,13 @@
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
@@ -1777,10 +1777,10 @@
         <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,13 +1794,13 @@
         <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="F26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
@@ -1809,10 +1809,10 @@
         <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1826,13 +1826,13 @@
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
@@ -1841,10 +1841,10 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1858,13 +1858,13 @@
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
@@ -1873,10 +1873,10 @@
         <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G29" t="s">
         <v>21</v>
@@ -1905,10 +1905,10 @@
         <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1922,13 +1922,13 @@
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G30" t="s">
         <v>21</v>
@@ -1937,10 +1937,10 @@
         <v>13</v>
       </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1954,13 +1954,13 @@
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
@@ -1969,10 +1969,10 @@
         <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1986,13 +1986,13 @@
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
@@ -2001,10 +2001,10 @@
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2018,13 +2018,13 @@
         <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
@@ -2033,10 +2033,10 @@
         <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2050,13 +2050,13 @@
         <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G34" t="s">
         <v>21</v>
@@ -2065,10 +2065,10 @@
         <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2082,13 +2082,13 @@
         <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G35" t="s">
         <v>21</v>
@@ -2097,10 +2097,10 @@
         <v>13</v>
       </c>
       <c r="J35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2114,13 +2114,13 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
@@ -2129,10 +2129,10 @@
         <v>13</v>
       </c>
       <c r="J36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2146,13 +2146,13 @@
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G37" t="s">
         <v>21</v>
@@ -2161,10 +2161,10 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2178,13 +2178,13 @@
         <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
@@ -2193,10 +2193,10 @@
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2210,13 +2210,13 @@
         <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
@@ -2225,10 +2225,10 @@
         <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2242,13 +2242,13 @@
         <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40" t="s">
         <v>21</v>
@@ -2257,10 +2257,10 @@
         <v>13</v>
       </c>
       <c r="J40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K40" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2274,13 +2274,13 @@
         <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
@@ -2289,10 +2289,10 @@
         <v>13</v>
       </c>
       <c r="J41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2318,10 +2318,10 @@
         <v>73</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K42" t="s">
         <v>74</v>
@@ -2350,10 +2350,10 @@
         <v>53</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I43" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K43" t="s">
         <v>77</v>
@@ -2382,7 +2382,7 @@
         <v>93</v>
       </c>
       <c r="I44" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K44" t="s">
         <v>85</v>
@@ -2411,10 +2411,10 @@
         <v>53</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K45" t="s">
         <v>76</v>
@@ -2443,10 +2443,10 @@
         <v>53</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K46" t="s">
         <v>78</v>
@@ -2475,10 +2475,10 @@
         <v>53</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K47" t="s">
         <v>79</v>
@@ -2495,20 +2495,20 @@
         <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2534,10 +2534,10 @@
         <v>53</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K49" t="s">
         <v>87</v>
@@ -2566,10 +2566,10 @@
         <v>53</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I50" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K50" t="s">
         <v>88</v>
@@ -2598,10 +2598,10 @@
         <v>53</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K51" t="s">
         <v>92</v>
@@ -2630,10 +2630,10 @@
         <v>53</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I52" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K52" t="s">
         <v>91</v>
@@ -2656,13 +2656,13 @@
         <v>97</v>
       </c>
       <c r="F53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2688,13 +2688,13 @@
         <v>98</v>
       </c>
       <c r="F54" t="s">
+        <v>101</v>
+      </c>
+      <c r="G54" t="s">
         <v>102</v>
       </c>
-      <c r="G54" t="s">
-        <v>103</v>
-      </c>
       <c r="H54" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2720,13 +2720,13 @@
         <v>99</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2746,16 +2746,16 @@
         <v>95</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G56" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2775,16 +2775,16 @@
         <v>95</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F57" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G57" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2804,16 +2804,16 @@
         <v>95</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F58" t="s">
+        <v>190</v>
+      </c>
+      <c r="G58" t="s">
         <v>193</v>
-      </c>
-      <c r="G58" t="s">
-        <v>196</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2833,16 +2833,16 @@
         <v>95</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F59" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G59" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2859,22 +2859,22 @@
         <v>94</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2891,22 +2891,22 @@
         <v>94</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F61" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" t="s">
         <v>116</v>
       </c>
-      <c r="G61" t="s">
-        <v>117</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2923,22 +2923,22 @@
         <v>94</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I62" t="s">
         <v>13</v>
@@ -2955,19 +2955,19 @@
         <v>94</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" t="s">
+        <v>115</v>
+      </c>
+      <c r="G63" t="s">
         <v>120</v>
-      </c>
-      <c r="F63" t="s">
-        <v>116</v>
-      </c>
-      <c r="G63" t="s">
-        <v>121</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" t="s">
@@ -2985,28 +2985,28 @@
         <v>94</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F64" t="s">
         <v>123</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>124</v>
       </c>
-      <c r="G64" t="s">
-        <v>125</v>
-      </c>
       <c r="H64" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I64" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="J64" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3131,62 +3131,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3206,27 +3206,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update banner text, remove enabler 1, fix SDQ rounding 1dp, correct UASC via metadata correction
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21F46AB-ACA6-4428-B6E2-DCB95B8A2026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832C9793-1034-4774-BCF5-96F37344070E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="345" yWindow="4335" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="205">
   <si>
     <t>tab_name</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>list(role = "Total", breakdown = "Non-white")</t>
+  </si>
+  <si>
+    <t>combined_cla_31_march_data</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1215,7 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1258,13 +1261,13 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>204</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed bug with stat_prev == stat_current, fixed CS Share
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832C9793-1034-4774-BCF5-96F37344070E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AE5E3D-6FBF-4016-A02B-BE5FBF8E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4335" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="17895" yWindow="4545" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -644,9 +644,6 @@
     <t>minus_cla_share</t>
   </si>
   <si>
-    <t>cs_share</t>
-  </si>
-  <si>
     <t>list(role = 'Total', breakdown = 'Non-white')</t>
   </si>
   <si>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>combined_cla_31_march_data</t>
+  </si>
+  <si>
+    <t>CS Share</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1261,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -2662,7 +2662,7 @@
         <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>188</v>
@@ -3006,10 +3006,10 @@
         <v>188</v>
       </c>
       <c r="I64" t="s">
+        <v>201</v>
+      </c>
+      <c r="J64" t="s">
         <v>202</v>
-      </c>
-      <c r="J64" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement assessment factors caused by data issue in metadata file
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AE5E3D-6FBF-4016-A02B-BE5FBF8E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8793FF-ED97-4541-82C9-53B6F0ADDF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="4545" windowWidth="25380" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="14025" yWindow="4680" windowWidth="36795" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="208">
   <si>
     <t>tab_name</t>
   </si>
@@ -263,24 +263,9 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t>list("placement_stability" = "With 3 or more placements during the year")</t>
-  </si>
-  <si>
     <t>placement_data</t>
   </si>
   <si>
-    <t>list("characteristic" = "Foster placements")</t>
-  </si>
-  <si>
-    <t>list("characteristic" = "Placed more than 20 miles from home")</t>
-  </si>
-  <si>
-    <t>list("characteristic" = "Secure homes and children's homes")</t>
-  </si>
-  <si>
-    <t>list("characteristic" = "Independent and semi-independent living arrangements/supported accommodation")</t>
-  </si>
-  <si>
     <t>Quality of life for care experienced people</t>
   </si>
   <si>
@@ -296,30 +281,15 @@
     <t>Care leavers in accommodation considered suitable (19 to 21 years)</t>
   </si>
   <si>
-    <t>list("age_start_poc" = "Total (all ages)")</t>
-  </si>
-  <si>
     <t>placement_order_match_data</t>
   </si>
   <si>
-    <t>list(age = "17 to 18 years", activity = "Total in education, employment or training" )</t>
-  </si>
-  <si>
-    <t>list(age = "19 to 21 years", activity = "Total in education, employment or training" )</t>
-  </si>
-  <si>
     <t>care_leavers_activity_data</t>
   </si>
   <si>
     <t>care_leavers_accommodation_data</t>
   </si>
   <si>
-    <t>list(age = "19 to 21 years", accommodation_suitability = "Accommodation considered suitable")</t>
-  </si>
-  <si>
-    <t>list(age = "17 to 18 years", accommodation_suitability = "Accommodation considered suitable")</t>
-  </si>
-  <si>
     <t>months</t>
   </si>
   <si>
@@ -470,63 +440,12 @@
     <t>Sexual Abuse unknown</t>
   </si>
   <si>
-    <t>list("assessment_factor" = "Domestic Abuse child")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Domestic Abuse parent")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Domestic Abuse person")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Emotional Abuse")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Faith linked abuse")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Neglect")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Physical Abuse adult on child")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Physical Abuse child on child")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Physical Abuse unknown")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Sexual Abuse adult on child")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Sexual Abuse child on child")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Sexual Abuse unknown")</t>
-  </si>
-  <si>
     <t>assessment_factors</t>
   </si>
   <si>
     <t>Harms outside the home</t>
   </si>
   <si>
-    <t>list("assessment_factor" = "Child criminal exploitation")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Child sexual exploitation")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Gangs")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Going missing")</t>
-  </si>
-  <si>
-    <t>list("assessment_factor" = "Trafficking")</t>
-  </si>
-  <si>
     <t>list('population_count' = 'Children starting to be looked after each year')</t>
   </si>
   <si>
@@ -593,9 +512,6 @@
     <t>assessment_factor</t>
   </si>
   <si>
-    <t>dimensional_filter_backup</t>
-  </si>
-  <si>
     <t>list('characteristic' = "Secure homes and children's homes")</t>
   </si>
   <si>
@@ -654,6 +570,99 @@
   </si>
   <si>
     <t>CS Share</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Neglect')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Gangs')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Trafficking')</t>
+  </si>
+  <si>
+    <t>Domestic Abuse child</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Domestic Abuse child')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Domestic Abuse parent')</t>
+  </si>
+  <si>
+    <t>Domestic Abuse parent</t>
+  </si>
+  <si>
+    <t>Domestic Abuse person</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Domestic Abuse person')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Emotional Abuse')</t>
+  </si>
+  <si>
+    <t>Emotional Abuse</t>
+  </si>
+  <si>
+    <t>Faith linked abuse</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Physical Abuse adult on child')</t>
+  </si>
+  <si>
+    <t>Physical Abuse adult on child</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Physical Abuse child on child')</t>
+  </si>
+  <si>
+    <t>Physical Abuse child on child</t>
+  </si>
+  <si>
+    <t>Physical Abuse unknown</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Physical Abuse unknown')</t>
+  </si>
+  <si>
+    <t>Sexual Abuse adult on child</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Sexual Abuse adult on child')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Sexual Abuse unknown')</t>
+  </si>
+  <si>
+    <t>Sexual Abuse unknown</t>
+  </si>
+  <si>
+    <t>Child criminal exploitation</t>
+  </si>
+  <si>
+    <t>Child sexual exploitation</t>
+  </si>
+  <si>
+    <t>Going missing</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Going missing')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Child sexual exploitation')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Faith linked abuse')</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Sexual Abuse child on child')</t>
+  </si>
+  <si>
+    <t>Sexual Abuse child on child</t>
+  </si>
+  <si>
+    <t>list('assessment_factor' = 'Child criminal exploitation')</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1085,7 @@
     <col min="9" max="10" width="81.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1099,19 +1108,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1160,13 +1166,13 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1189,10 +1195,10 @@
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1215,10 +1221,10 @@
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1241,10 +1247,10 @@
         <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1261,16 +1267,16 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1293,13 +1299,13 @@
         <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1322,13 +1328,13 @@
         <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1351,13 +1357,13 @@
         <v>35</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1380,13 +1386,13 @@
         <v>36</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1409,13 +1415,13 @@
         <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1438,13 +1444,13 @@
         <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1467,13 +1473,13 @@
         <v>47</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1496,13 +1502,13 @@
         <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1525,13 +1531,13 @@
         <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1555,10 +1561,10 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1582,10 +1588,10 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1609,10 +1615,10 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1635,13 +1641,13 @@
         <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1664,13 +1670,13 @@
         <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I21" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1693,13 +1699,13 @@
         <v>58</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1722,13 +1728,13 @@
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1765,28 +1771,25 @@
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G25" t="s">
         <v>21</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
       <c r="J25" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1797,28 +1800,25 @@
         <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G26" t="s">
         <v>21</v>
       </c>
       <c r="I26" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="J26" t="s">
-        <v>132</v>
-      </c>
-      <c r="K26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1829,28 +1829,25 @@
         <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" t="s">
         <v>133</v>
-      </c>
-      <c r="F27" t="s">
-        <v>155</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
       <c r="J27" t="s">
-        <v>133</v>
-      </c>
-      <c r="K27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1861,28 +1858,25 @@
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G28" t="s">
         <v>21</v>
       </c>
       <c r="I28" t="s">
-        <v>13</v>
+        <v>186</v>
       </c>
       <c r="J28" t="s">
-        <v>134</v>
-      </c>
-      <c r="K28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1893,28 +1887,25 @@
         <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F29" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G29" t="s">
         <v>21</v>
       </c>
       <c r="I29" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="J29" t="s">
-        <v>135</v>
-      </c>
-      <c r="K29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1925,28 +1916,25 @@
         <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G30" t="s">
         <v>21</v>
       </c>
       <c r="I30" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="J30" t="s">
-        <v>136</v>
-      </c>
-      <c r="K30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1957,28 +1945,25 @@
         <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F31" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G31" t="s">
         <v>21</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>189</v>
       </c>
       <c r="J31" t="s">
-        <v>137</v>
-      </c>
-      <c r="K31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1989,28 +1974,25 @@
         <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F32" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G32" t="s">
         <v>21</v>
       </c>
       <c r="I32" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="J32" t="s">
-        <v>138</v>
-      </c>
-      <c r="K32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2021,28 +2003,25 @@
         <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="F33" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G33" t="s">
         <v>21</v>
       </c>
       <c r="I33" t="s">
-        <v>13</v>
+        <v>194</v>
       </c>
       <c r="J33" t="s">
-        <v>139</v>
-      </c>
-      <c r="K33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2053,28 +2032,25 @@
         <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G34" t="s">
         <v>21</v>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="J34" t="s">
-        <v>140</v>
-      </c>
-      <c r="K34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2085,28 +2061,25 @@
         <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G35" t="s">
         <v>21</v>
       </c>
       <c r="I35" t="s">
-        <v>13</v>
+        <v>205</v>
       </c>
       <c r="J35" t="s">
-        <v>141</v>
-      </c>
-      <c r="K35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2117,28 +2090,25 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F36" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G36" t="s">
         <v>21</v>
       </c>
       <c r="I36" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="J36" t="s">
-        <v>142</v>
-      </c>
-      <c r="K36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2149,28 +2119,25 @@
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G37" t="s">
         <v>21</v>
       </c>
       <c r="I37" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="J37" t="s">
-        <v>129</v>
-      </c>
-      <c r="K37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2181,28 +2148,25 @@
         <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F38" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G38" t="s">
         <v>21</v>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="J38" t="s">
-        <v>126</v>
-      </c>
-      <c r="K38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2213,28 +2177,25 @@
         <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G39" t="s">
         <v>21</v>
       </c>
       <c r="I39" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="J39" t="s">
-        <v>128</v>
-      </c>
-      <c r="K39" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2245,28 +2206,25 @@
         <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F40" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G40" t="s">
         <v>21</v>
       </c>
       <c r="I40" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="J40" t="s">
-        <v>125</v>
-      </c>
-      <c r="K40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2277,28 +2235,25 @@
         <v>54</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="F41" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G41" t="s">
         <v>21</v>
       </c>
       <c r="I41" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="J41" t="s">
-        <v>127</v>
-      </c>
-      <c r="K41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2321,16 +2276,13 @@
         <v>73</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I42" t="s">
-        <v>174</v>
-      </c>
-      <c r="K42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2347,22 +2299,19 @@
         <v>67</v>
       </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43" t="s">
         <v>53</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I43" t="s">
-        <v>175</v>
-      </c>
-      <c r="K43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2379,19 +2328,16 @@
         <v>68</v>
       </c>
       <c r="F44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G44" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I44" t="s">
-        <v>176</v>
-      </c>
-      <c r="K44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2408,22 +2354,19 @@
         <v>69</v>
       </c>
       <c r="F45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G45" t="s">
         <v>53</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I45" t="s">
-        <v>177</v>
-      </c>
-      <c r="K45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2440,22 +2383,19 @@
         <v>70</v>
       </c>
       <c r="F46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G46" t="s">
         <v>53</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I46" t="s">
-        <v>185</v>
-      </c>
-      <c r="K46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2472,22 +2412,19 @@
         <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G47" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I47" t="s">
-        <v>178</v>
-      </c>
-      <c r="K47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2498,23 +2435,23 @@
         <v>65</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2525,28 +2462,25 @@
         <v>65</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" t="s">
         <v>81</v>
-      </c>
-      <c r="F49" t="s">
-        <v>89</v>
       </c>
       <c r="G49" t="s">
         <v>53</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I49" t="s">
-        <v>179</v>
-      </c>
-      <c r="K49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2557,28 +2491,25 @@
         <v>65</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F50" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G50" t="s">
         <v>53</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I50" t="s">
-        <v>180</v>
-      </c>
-      <c r="K50" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2589,28 +2520,25 @@
         <v>65</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G51" t="s">
         <v>53</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I51" t="s">
-        <v>181</v>
-      </c>
-      <c r="K51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2621,51 +2549,48 @@
         <v>65</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G52" t="s">
         <v>53</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I52" t="s">
-        <v>182</v>
-      </c>
-      <c r="K52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F53" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G53" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2674,30 +2599,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F54" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G54" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2706,30 +2631,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F55" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G55" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2738,27 +2663,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="F56" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="G56" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2767,27 +2692,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F57" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="G57" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2796,27 +2721,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E58" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F58" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="G58" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2825,27 +2750,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F59" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="G59" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2854,30 +2779,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F60" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G60" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2886,30 +2811,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F61" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G61" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2918,30 +2843,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F62" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G62" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I62" t="s">
         <v>13</v>
@@ -2950,27 +2875,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="F63" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G63" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" t="s">
@@ -2980,36 +2905,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F64" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G64" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="I64" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="J64" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3134,62 +3059,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3209,27 +3134,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated metadata to add rate per 10k for assessment factors, fixed the minus numeric issue with assessment factors
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8793FF-ED97-4541-82C9-53B6F0ADDF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24D1481-9530-4C19-BF56-52FBE94BE29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14025" yWindow="4680" windowWidth="36795" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="226">
   <si>
     <t>tab_name</t>
   </si>
@@ -663,6 +663,60 @@
   </si>
   <si>
     <t>list('assessment_factor' = 'Child criminal exploitation')</t>
+  </si>
+  <si>
+    <t>rate_per_10000_char</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse parent per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse person per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Emotional Abuse per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Faith linked abuse per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Neglect per 10k</t>
+  </si>
+  <si>
+    <t>Rate of  Physical Abuse adult on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse child on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse unknown per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse adult on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse child on child per10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse unknown per10k</t>
+  </si>
+  <si>
+    <t>Rate of Child criminal exploitation per10k</t>
+  </si>
+  <si>
+    <t>Rate of Child sexual exploitation per10k</t>
+  </si>
+  <si>
+    <t>Rate of Gangs per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Going missing per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Trafficking per 10k</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1808,7 @@
         <v>62</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I24" t="s">
         <v>13</v>
@@ -1774,13 +1828,13 @@
         <v>120</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="F25" t="s">
         <v>133</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I25" t="s">
         <v>181</v>
@@ -1803,13 +1857,13 @@
         <v>120</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="F26" t="s">
         <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I26" t="s">
         <v>182</v>
@@ -1832,13 +1886,13 @@
         <v>120</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>123</v>
+        <v>211</v>
       </c>
       <c r="F27" t="s">
         <v>133</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I27" t="s">
         <v>185</v>
@@ -1861,13 +1915,13 @@
         <v>120</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
       <c r="F28" t="s">
         <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I28" t="s">
         <v>186</v>
@@ -1890,13 +1944,13 @@
         <v>120</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
       <c r="F29" t="s">
         <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I29" t="s">
         <v>204</v>
@@ -1919,13 +1973,13 @@
         <v>120</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I30" t="s">
         <v>177</v>
@@ -1948,13 +2002,13 @@
         <v>120</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
         <v>133</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I31" t="s">
         <v>189</v>
@@ -1977,13 +2031,13 @@
         <v>120</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="F32" t="s">
         <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I32" t="s">
         <v>191</v>
@@ -2006,13 +2060,13 @@
         <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="F33" t="s">
         <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I33" t="s">
         <v>194</v>
@@ -2035,13 +2089,13 @@
         <v>120</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="F34" t="s">
         <v>133</v>
       </c>
       <c r="G34" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I34" t="s">
         <v>196</v>
@@ -2064,13 +2118,13 @@
         <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
         <v>133</v>
       </c>
       <c r="G35" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I35" t="s">
         <v>205</v>
@@ -2093,13 +2147,13 @@
         <v>120</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="F36" t="s">
         <v>133</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I36" t="s">
         <v>197</v>
@@ -2122,13 +2176,13 @@
         <v>134</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>119</v>
+        <v>221</v>
       </c>
       <c r="F37" t="s">
         <v>133</v>
       </c>
       <c r="G37" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I37" t="s">
         <v>207</v>
@@ -2151,13 +2205,13 @@
         <v>134</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="F38" t="s">
         <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I38" t="s">
         <v>203</v>
@@ -2180,13 +2234,13 @@
         <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="F39" t="s">
         <v>133</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I39" t="s">
         <v>178</v>
@@ -2209,13 +2263,13 @@
         <v>134</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>115</v>
+        <v>224</v>
       </c>
       <c r="F40" t="s">
         <v>133</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I40" t="s">
         <v>202</v>
@@ -2238,13 +2292,13 @@
         <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>117</v>
+        <v>225</v>
       </c>
       <c r="F41" t="s">
         <v>133</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
+        <v>208</v>
       </c>
       <c r="I41" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Updated metadata to add rate per 10k for assessment factors, fixed the minus numeric issue with assessment factors. Fixed Excliding CLA share
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8793FF-ED97-4541-82C9-53B6F0ADDF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869415F-8076-44D6-A2CE-7E440EDF1650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14025" yWindow="4680" windowWidth="36795" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="226">
   <si>
     <t>tab_name</t>
   </si>
@@ -557,9 +557,6 @@
     <t>wellbeing_sdq_data</t>
   </si>
   <si>
-    <t>minus_cla_share</t>
-  </si>
-  <si>
     <t>list(role = 'Total', breakdown = 'Non-white')</t>
   </si>
   <si>
@@ -663,6 +660,63 @@
   </si>
   <si>
     <t>list('assessment_factor' = 'Child criminal exploitation')</t>
+  </si>
+  <si>
+    <t>rate_per_10000_char</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse parent per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse person per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Emotional Abuse per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Faith linked abuse per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Neglect per 10k</t>
+  </si>
+  <si>
+    <t>Rate of  Physical Abuse adult on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse child on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse unknown per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse adult on child per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse child on child per10k</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse unknown per10k</t>
+  </si>
+  <si>
+    <t>Rate of Child criminal exploitation per10k</t>
+  </si>
+  <si>
+    <t>Rate of Child sexual exploitation per10k</t>
+  </si>
+  <si>
+    <t>Rate of Gangs per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Going missing per 10k</t>
+  </si>
+  <si>
+    <t>Rate of Trafficking per 10k</t>
+  </si>
+  <si>
+    <t>Excluding CLA Share</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -1774,19 +1828,19 @@
         <v>120</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="F25" t="s">
         <v>133</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1803,19 +1857,19 @@
         <v>120</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>122</v>
+        <v>209</v>
       </c>
       <c r="F26" t="s">
         <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I26" t="s">
+        <v>181</v>
+      </c>
+      <c r="J26" t="s">
         <v>182</v>
-      </c>
-      <c r="J26" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1832,19 +1886,19 @@
         <v>120</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="F27" t="s">
         <v>133</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1861,19 +1915,19 @@
         <v>120</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="F28" t="s">
         <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" t="s">
         <v>186</v>
-      </c>
-      <c r="J28" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1890,19 +1944,19 @@
         <v>120</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="F29" t="s">
         <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1919,16 +1973,16 @@
         <v>120</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="F30" t="s">
         <v>133</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J30" t="s">
         <v>126</v>
@@ -1948,19 +2002,19 @@
         <v>120</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>127</v>
+        <v>214</v>
       </c>
       <c r="F31" t="s">
         <v>133</v>
       </c>
       <c r="G31" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I31" t="s">
+        <v>188</v>
+      </c>
+      <c r="J31" t="s">
         <v>189</v>
-      </c>
-      <c r="J31" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1977,19 +2031,19 @@
         <v>120</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>128</v>
+        <v>215</v>
       </c>
       <c r="F32" t="s">
         <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I32" t="s">
+        <v>190</v>
+      </c>
+      <c r="J32" t="s">
         <v>191</v>
-      </c>
-      <c r="J32" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2006,19 +2060,19 @@
         <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>129</v>
+        <v>216</v>
       </c>
       <c r="F33" t="s">
         <v>133</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2035,19 +2089,19 @@
         <v>120</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>130</v>
+        <v>217</v>
       </c>
       <c r="F34" t="s">
         <v>133</v>
       </c>
       <c r="G34" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2064,19 +2118,19 @@
         <v>120</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="F35" t="s">
         <v>133</v>
       </c>
       <c r="G35" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I35" t="s">
+        <v>204</v>
+      </c>
+      <c r="J35" t="s">
         <v>205</v>
-      </c>
-      <c r="J35" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2093,19 +2147,19 @@
         <v>120</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="F36" t="s">
         <v>133</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I36" t="s">
+        <v>196</v>
+      </c>
+      <c r="J36" t="s">
         <v>197</v>
-      </c>
-      <c r="J36" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2122,19 +2176,19 @@
         <v>134</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>119</v>
+        <v>220</v>
       </c>
       <c r="F37" t="s">
         <v>133</v>
       </c>
       <c r="G37" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2151,19 +2205,19 @@
         <v>134</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="F38" t="s">
         <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2180,16 +2234,16 @@
         <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="F39" t="s">
         <v>133</v>
       </c>
       <c r="G39" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J39" t="s">
         <v>118</v>
@@ -2209,19 +2263,19 @@
         <v>134</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>115</v>
+        <v>223</v>
       </c>
       <c r="F40" t="s">
         <v>133</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2238,16 +2292,16 @@
         <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>117</v>
+        <v>224</v>
       </c>
       <c r="F41" t="s">
         <v>133</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
+        <v>207</v>
       </c>
       <c r="I41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J41" t="s">
         <v>117</v>
@@ -2587,7 +2641,7 @@
         <v>90</v>
       </c>
       <c r="G53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>160</v>
@@ -2651,7 +2705,7 @@
         <v>93</v>
       </c>
       <c r="G55" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>160</v>
@@ -2931,10 +2985,10 @@
         <v>160</v>
       </c>
       <c r="I64" t="s">
+        <v>172</v>
+      </c>
+      <c r="J64" t="s">
         <v>173</v>
-      </c>
-      <c r="J64" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add na to months to adoption, fix bug Yorkshire and The Humber assessment factor bar chart causing error, cleaned Ofsted mapping for County Durham which fixed the other issues.
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2445346-C375-4CCB-B6F0-5C9133ED2BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BE6AB0-A3BE-4215-84FA-0E72AA85ACCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14025" yWindow="4680" windowWidth="36795" windowHeight="15795" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="227">
   <si>
     <t>tab_name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Family stability</t>
   </si>
   <si>
-    <t>Rate of children to be looked after</t>
-  </si>
-  <si>
     <t>cla_rates</t>
   </si>
   <si>
@@ -110,15 +107,9 @@
     <t>combined_cla_data</t>
   </si>
   <si>
-    <t>Rate of children starting to be looked after who were UASC per 10k</t>
-  </si>
-  <si>
     <t>Rate of children looked after on 31 March who were UASC, per 10,000 children</t>
   </si>
   <si>
-    <t>Rate of children starting to be looked after on 31 March per 10k</t>
-  </si>
-  <si>
     <t>placement_per_10000</t>
   </si>
   <si>
@@ -230,9 +221,6 @@
     <t>hospital_admissions</t>
   </si>
   <si>
-    <t>Hospital admissions caused by unintentional and deliberate injuries to children and young people (0 to 14 years)</t>
-  </si>
-  <si>
     <t>% CLA on 31 March with 3 or more placements during the year</t>
   </si>
   <si>
@@ -665,58 +653,73 @@
     <t>rate_per_10000_char</t>
   </si>
   <si>
-    <t>Rate of Domestic Abuse child per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Domestic Abuse parent per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Domestic Abuse person per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Emotional Abuse per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Faith linked abuse per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Neglect per 10k</t>
-  </si>
-  <si>
-    <t>Rate of  Physical Abuse adult on child per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Physical Abuse child on child per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Physical Abuse unknown per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Sexual Abuse adult on child per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Sexual Abuse child on child per10k</t>
-  </si>
-  <si>
-    <t>Rate of Sexual Abuse unknown per10k</t>
-  </si>
-  <si>
-    <t>Rate of Child criminal exploitation per10k</t>
-  </si>
-  <si>
-    <t>Rate of Child sexual exploitation per10k</t>
-  </si>
-  <si>
-    <t>Rate of Gangs per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Going missing per 10k</t>
-  </si>
-  <si>
-    <t>Rate of Trafficking per 10k</t>
-  </si>
-  <si>
     <t>Excluding CLA Share</t>
+  </si>
+  <si>
+    <t>Rate of children in need, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of children starting to be looked after who were UASC, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of children starting to be looked after on 31 March, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse child, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse parent, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Domestic Abuse person, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Emotional Abuse, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Faith linked abuse, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Neglect, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of  Physical Abuse adult on child, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse child on child, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Physical Abuse unknown, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse adult on child, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Gangs, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Going missing, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Trafficking, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse child on child, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Sexual Abuse unknown, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Child criminal exploitation, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Child sexual exploitation, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of children to be looked after, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of Hospital admissions caused by unintentional and deliberate injuries to children and young people (0 to 14 years), per 10,000 children</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1162,13 +1165,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1185,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1220,7 +1223,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -1240,16 +1243,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1266,16 +1269,16 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
       <c r="I5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1292,16 +1295,16 @@
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>207</v>
       </c>
       <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
       <c r="I6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1318,16 +1321,16 @@
         <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1341,22 +1344,22 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,22 +1373,22 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1399,22 +1402,22 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,22 +1431,22 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,22 +1460,22 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1486,22 +1489,22 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1515,22 +1518,22 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1544,22 +1547,22 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1573,22 +1576,22 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1602,20 +1605,20 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" t="s">
         <v>43</v>
-      </c>
-      <c r="F17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1629,20 +1632,20 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1656,20 +1659,20 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" t="s">
-        <v>42</v>
-      </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1680,25 +1683,25 @@
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" t="s">
         <v>50</v>
       </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1709,25 +1712,25 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" t="s">
-        <v>52</v>
-      </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1738,22 +1741,22 @@
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1767,22 +1770,22 @@
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" t="s">
         <v>57</v>
       </c>
-      <c r="F23" t="s">
-        <v>60</v>
-      </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1796,19 +1799,19 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>63</v>
+        <v>226</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" t="s">
         <v>13</v>
@@ -1822,25 +1825,25 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>208</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G25" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="J25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1851,25 +1854,25 @@
         <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>209</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I26" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J26" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1880,25 +1883,25 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>210</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G27" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I27" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J27" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1909,25 +1912,25 @@
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I28" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J28" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1938,25 +1941,25 @@
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>212</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G29" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I29" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J29" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1967,25 +1970,25 @@
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1996,25 +1999,25 @@
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>214</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G31" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I31" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2025,25 +2028,25 @@
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G32" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J32" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2054,25 +2057,25 @@
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>216</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G33" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I33" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J33" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2083,25 +2086,25 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>217</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I34" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J34" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2112,25 +2115,25 @@
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F35" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I35" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J35" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2141,25 +2144,25 @@
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I36" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2170,25 +2173,25 @@
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I37" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J37" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2199,25 +2202,25 @@
         <v>6</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G38" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I38" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J38" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2228,25 +2231,25 @@
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G39" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J39" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2257,25 +2260,25 @@
         <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I40" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J40" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2286,25 +2289,25 @@
         <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F41" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G41" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I41" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2315,25 +2318,25 @@
         <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F42" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I42" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2344,25 +2347,25 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,22 +2376,22 @@
         <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F44" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G44" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2399,25 +2402,25 @@
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I45" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2428,25 +2431,25 @@
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" t="s">
         <v>70</v>
       </c>
-      <c r="F46" t="s">
-        <v>74</v>
-      </c>
       <c r="G46" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I46" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2457,25 +2460,25 @@
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I47" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2486,23 +2489,23 @@
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2513,25 +2516,25 @@
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2542,25 +2545,25 @@
         <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" t="s">
         <v>77</v>
       </c>
-      <c r="F50" t="s">
-        <v>81</v>
-      </c>
       <c r="G50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I50" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2571,25 +2574,25 @@
         <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" t="s">
         <v>78</v>
       </c>
-      <c r="F51" t="s">
-        <v>82</v>
-      </c>
       <c r="G51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I51" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2600,25 +2603,25 @@
         <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I52" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2626,25 +2629,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F53" t="s">
-        <v>90</v>
-      </c>
       <c r="G53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2658,25 +2661,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" t="s">
+        <v>87</v>
+      </c>
+      <c r="G54" t="s">
         <v>88</v>
       </c>
-      <c r="F54" t="s">
-        <v>91</v>
-      </c>
-      <c r="G54" t="s">
-        <v>92</v>
-      </c>
       <c r="H54" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2690,25 +2693,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" t="s">
         <v>89</v>
       </c>
-      <c r="F55" t="s">
-        <v>93</v>
-      </c>
       <c r="G55" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2722,22 +2725,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F56" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G56" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2751,22 +2754,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F57" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2780,22 +2783,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G58" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2809,22 +2812,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F59" t="s">
+        <v>158</v>
+      </c>
+      <c r="G59" t="s">
         <v>162</v>
-      </c>
-      <c r="G59" t="s">
-        <v>166</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2838,25 +2841,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F60" t="s">
+        <v>101</v>
+      </c>
+      <c r="G60" t="s">
         <v>100</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F60" t="s">
-        <v>105</v>
-      </c>
-      <c r="G60" t="s">
-        <v>104</v>
-      </c>
       <c r="H60" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2870,25 +2873,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F61" t="s">
+        <v>101</v>
+      </c>
+      <c r="G61" t="s">
         <v>102</v>
       </c>
-      <c r="F61" t="s">
-        <v>105</v>
-      </c>
-      <c r="G61" t="s">
-        <v>106</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2902,25 +2905,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" t="s">
         <v>103</v>
       </c>
-      <c r="F62" t="s">
-        <v>105</v>
-      </c>
-      <c r="G62" t="s">
-        <v>107</v>
-      </c>
       <c r="H62" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I62" t="s">
         <v>13</v>
@@ -2934,22 +2937,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F63" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G63" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" t="s">
@@ -2964,31 +2967,31 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F64" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G64" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I64" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J64" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3113,62 +3116,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3188,27 +3191,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to metadata for the Family stability numbers to be right
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BE6AB0-A3BE-4215-84FA-0E72AA85ACCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69542F34-749A-4D55-B3CA-A8CF361F92F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="22540" windowHeight="14300" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="20" yWindow="260" windowWidth="22540" windowHeight="14300" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
-    <sheet name="Enablers" sheetId="2" r:id="rId2"/>
-    <sheet name="AF1" sheetId="4" r:id="rId3"/>
-    <sheet name="AF2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Enablers" sheetId="2" r:id="rId3"/>
+    <sheet name="AF1" sheetId="4" r:id="rId4"/>
+    <sheet name="AF2" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="227">
   <si>
     <t>tab_name</t>
   </si>
@@ -662,9 +663,6 @@
     <t>Rate of children starting to be looked after who were UASC, per 10,000 children</t>
   </si>
   <si>
-    <t>Rate of children starting to be looked after on 31 March, per 10,000 children</t>
-  </si>
-  <si>
     <t>Rate of Domestic Abuse child, per 10,000 children</t>
   </si>
   <si>
@@ -716,10 +714,13 @@
     <t>Rate of Child sexual exploitation, per 10,000 children</t>
   </si>
   <si>
-    <t>Rate of children to be looked after, per 10,000 children</t>
-  </si>
-  <si>
     <t>Rate of Hospital admissions caused by unintentional and deliberate injuries to children and young people (0 to 14 years), per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of children starting to be looked after, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Rate of children looked after on 31 March, per 10,000 children</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1253,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1268,17 +1269,17 @@
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>206</v>
+      <c r="E5" t="s">
+        <v>226</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1295,16 +1296,16 @@
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1805,7 +1806,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -1831,7 +1832,7 @@
         <v>116</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F25" t="s">
         <v>129</v>
@@ -1860,7 +1861,7 @@
         <v>116</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F26" t="s">
         <v>129</v>
@@ -1889,7 +1890,7 @@
         <v>116</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F27" t="s">
         <v>129</v>
@@ -1918,7 +1919,7 @@
         <v>116</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F28" t="s">
         <v>129</v>
@@ -1947,7 +1948,7 @@
         <v>116</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F29" t="s">
         <v>129</v>
@@ -1976,7 +1977,7 @@
         <v>116</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" t="s">
         <v>129</v>
@@ -2005,7 +2006,7 @@
         <v>116</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F31" t="s">
         <v>129</v>
@@ -2034,7 +2035,7 @@
         <v>116</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F32" t="s">
         <v>129</v>
@@ -2063,7 +2064,7 @@
         <v>116</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F33" t="s">
         <v>129</v>
@@ -2092,7 +2093,7 @@
         <v>116</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F34" t="s">
         <v>129</v>
@@ -2121,7 +2122,7 @@
         <v>116</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F35" t="s">
         <v>129</v>
@@ -2150,7 +2151,7 @@
         <v>116</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F36" t="s">
         <v>129</v>
@@ -2179,7 +2180,7 @@
         <v>130</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F37" t="s">
         <v>129</v>
@@ -2208,7 +2209,7 @@
         <v>130</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F38" t="s">
         <v>129</v>
@@ -2237,7 +2238,7 @@
         <v>130</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F39" t="s">
         <v>129</v>
@@ -2266,7 +2267,7 @@
         <v>130</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F40" t="s">
         <v>129</v>
@@ -2295,7 +2296,7 @@
         <v>130</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F41" t="s">
         <v>129</v>
@@ -3002,6 +3003,99 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DC0F8E-C32C-4B1C-ACBA-A8D3F1832886}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C47140-91E9-451A-99FE-1BE9D9143F8C}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -3104,7 +3198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0C6DD7-AE28-4F4A-942E-394E553C1677}">
   <dimension ref="A1:A12"/>
   <sheetViews>
@@ -3179,7 +3273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC51871E-4DD5-4CFF-9196-6C5CC871D99B}">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Ofsted headline boxes fixed and London added. Used a reactive data for the 4 boxes to simplify code. Corrected spending no cla stat neighbours
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69542F34-749A-4D55-B3CA-A8CF361F92F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06462549-9719-42FA-BBF4-F12C43C2BC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="260" windowWidth="22540" windowHeight="14300" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="45390" windowHeight="16785" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add median back into the column headers, remove conditional panels on enabler 2 for region combinations, removed full stop enabler 3, updated Summary page heading, fixed padding on table headers for summary page
</commit_message>
<xml_diff>
--- a/data-raw/summary_page_metadata.xlsx
+++ b/data-raw/summary_page_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06462549-9719-42FA-BBF4-F12C43C2BC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD586CA-F110-4285-AE43-29CAE35BF445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="3030" windowWidth="45390" windowHeight="16785" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
@@ -327,9 +327,6 @@
     <t>Number of local authorities with an Ofsted Leadership Rating of Inadequate</t>
   </si>
   <si>
-    <t>Enabler: The workforce is equipped and effective.</t>
-  </si>
-  <si>
     <t>Workforce stability</t>
   </si>
   <si>
@@ -721,6 +718,9 @@
   </si>
   <si>
     <t>Rate of children looked after on 31 March, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Enabler: The workforce is equipped and effective</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1166,13 +1166,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1224,7 +1224,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -1244,7 +1244,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1253,7 +1253,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -1279,7 +1279,7 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1296,7 +1296,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
@@ -1305,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1325,13 +1325,13 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1357,10 +1357,10 @@
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1386,10 +1386,10 @@
         <v>32</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1415,10 +1415,10 @@
         <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1444,10 +1444,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1473,10 +1473,10 @@
         <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1502,10 +1502,10 @@
         <v>33</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1531,10 +1531,10 @@
         <v>44</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1560,10 +1560,10 @@
         <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1589,10 +1589,10 @@
         <v>44</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1699,10 +1699,10 @@
         <v>50</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1728,10 +1728,10 @@
         <v>50</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1757,7 +1757,7 @@
         <v>55</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1786,7 +1786,7 @@
         <v>58</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1806,7 +1806,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -1829,22 +1829,22 @@
         <v>51</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1858,22 +1858,22 @@
         <v>51</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I26" t="s">
+        <v>176</v>
+      </c>
+      <c r="J26" t="s">
         <v>177</v>
-      </c>
-      <c r="J26" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1887,22 +1887,22 @@
         <v>51</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1916,22 +1916,22 @@
         <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I28" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" t="s">
         <v>181</v>
-      </c>
-      <c r="J28" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1945,22 +1945,22 @@
         <v>51</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1974,22 +1974,22 @@
         <v>51</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2003,22 +2003,22 @@
         <v>51</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I31" t="s">
+        <v>183</v>
+      </c>
+      <c r="J31" t="s">
         <v>184</v>
-      </c>
-      <c r="J31" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2032,22 +2032,22 @@
         <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I32" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" t="s">
         <v>186</v>
-      </c>
-      <c r="J32" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2061,22 +2061,22 @@
         <v>51</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2090,22 +2090,22 @@
         <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2119,22 +2119,22 @@
         <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I35" t="s">
+        <v>199</v>
+      </c>
+      <c r="J35" t="s">
         <v>200</v>
-      </c>
-      <c r="J35" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2148,22 +2148,22 @@
         <v>51</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I36" t="s">
+        <v>191</v>
+      </c>
+      <c r="J36" t="s">
         <v>192</v>
-      </c>
-      <c r="J36" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2177,22 +2177,22 @@
         <v>51</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,22 +2206,22 @@
         <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2235,22 +2235,22 @@
         <v>51</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2264,22 +2264,22 @@
         <v>51</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2293,22 +2293,22 @@
         <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2334,10 +2334,10 @@
         <v>69</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2363,10 +2363,10 @@
         <v>50</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
         <v>79</v>
       </c>
       <c r="I44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2418,10 +2418,10 @@
         <v>50</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2447,10 +2447,10 @@
         <v>50</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2476,10 +2476,10 @@
         <v>50</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2493,20 +2493,20 @@
         <v>61</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2532,10 +2532,10 @@
         <v>50</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2561,10 +2561,10 @@
         <v>50</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2590,10 +2590,10 @@
         <v>50</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2619,10 +2619,10 @@
         <v>50</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2645,10 +2645,10 @@
         <v>86</v>
       </c>
       <c r="G53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I53" t="s">
         <v>13</v>
@@ -2680,7 +2680,7 @@
         <v>88</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I54" t="s">
         <v>13</v>
@@ -2709,10 +2709,10 @@
         <v>89</v>
       </c>
       <c r="G55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I55" t="s">
         <v>13</v>
@@ -2738,10 +2738,10 @@
         <v>90</v>
       </c>
       <c r="F56" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56" t="s">
         <v>158</v>
-      </c>
-      <c r="G56" t="s">
-        <v>159</v>
       </c>
       <c r="I56" t="s">
         <v>13</v>
@@ -2767,10 +2767,10 @@
         <v>92</v>
       </c>
       <c r="F57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I57" t="s">
         <v>13</v>
@@ -2796,10 +2796,10 @@
         <v>93</v>
       </c>
       <c r="F58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I58" t="s">
         <v>13</v>
@@ -2825,10 +2825,10 @@
         <v>94</v>
       </c>
       <c r="F59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I59" t="s">
         <v>13</v>
@@ -2845,22 +2845,22 @@
         <v>80</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I60" t="s">
         <v>13</v>
@@ -2877,22 +2877,22 @@
         <v>80</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F61" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" t="s">
         <v>101</v>
       </c>
-      <c r="G61" t="s">
-        <v>102</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -2909,22 +2909,22 @@
         <v>80</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I62" t="s">
         <v>13</v>
@@ -2941,19 +2941,19 @@
         <v>80</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" t="s">
         <v>105</v>
-      </c>
-      <c r="F63" t="s">
-        <v>101</v>
-      </c>
-      <c r="G63" t="s">
-        <v>106</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" t="s">
@@ -2971,28 +2971,28 @@
         <v>80</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="F64" t="s">
         <v>108</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>109</v>
       </c>
-      <c r="G64" t="s">
-        <v>110</v>
-      </c>
       <c r="H64" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I64" t="s">
+        <v>167</v>
+      </c>
+      <c r="J64" t="s">
         <v>168</v>
-      </c>
-      <c r="J64" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3022,7 +3022,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -3031,7 +3031,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3048,7 +3048,7 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -3065,7 +3065,7 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3076,18 +3076,18 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3210,62 +3210,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3285,27 +3285,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>